<commit_message>
Panel: Systemzeit-Informationen, Geräte-Informationen und Aktuelle Störungen
</commit_message>
<xml_diff>
--- a/Übersicht der Funktionen von Mikrocontroller und Kommunikationsmodul.xlsx
+++ b/Übersicht der Funktionen von Mikrocontroller und Kommunikationsmodul.xlsx
@@ -315,6 +315,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,11 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -637,7 +637,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,30 +658,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="12" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
@@ -735,13 +735,13 @@
       <c r="G3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="11" t="s">
         <v>26</v>
       </c>
       <c r="K3" t="s">
@@ -750,7 +750,7 @@
       <c r="L3" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -776,13 +776,13 @@
       <c r="G4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="11" t="s">
         <v>27</v>
       </c>
       <c r="K4" t="s">
@@ -817,16 +817,16 @@
       <c r="G5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -850,16 +850,16 @@
       <c r="G6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="11" t="s">
         <v>40</v>
       </c>
     </row>
@@ -882,10 +882,10 @@
         <v>43</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -906,10 +906,10 @@
         <v>44</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="11" t="s">
         <v>62</v>
       </c>
     </row>
@@ -930,10 +930,10 @@
         <v>45</v>
       </c>
       <c r="I9" s="5"/>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="14" t="s">
+      <c r="L9" s="11" t="s">
         <v>46</v>
       </c>
     </row>
@@ -949,7 +949,7 @@
       <c r="G10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="11" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update, Sprache und Kalibrierung
</commit_message>
<xml_diff>
--- a/Übersicht der Funktionen von Mikrocontroller und Kommunikationsmodul.xlsx
+++ b/Übersicht der Funktionen von Mikrocontroller und Kommunikationsmodul.xlsx
@@ -637,7 +637,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +963,7 @@
       <c r="G11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -977,7 +977,7 @@
       <c r="G12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="11" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>